<commit_message>
new version of script.py for the new input files
</commit_message>
<xml_diff>
--- a/data/data_table.xlsx
+++ b/data/data_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kucing\opencitations\oc_dmp\oc-dmp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391CF66-BD10-477B-95E2-167B8BEDA322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFA354F-2E12-418C-AE4C-921B35353FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main data table" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -631,6 +631,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -891,8 +895,9 @@
   </sheetPr>
   <dimension ref="A1:CF98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1684,7 +1689,7 @@
       </c>
     </row>
     <row r="4" spans="1:84" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B4" s="5"/>
@@ -1757,7 +1762,7 @@
       </c>
       <c r="Z4" s="11"/>
       <c r="AA4" s="21" t="str">
-        <f t="shared" ref="AA3:AC34" si="5">IF($L4="Software","","N/A")</f>
+        <f t="shared" ref="AA4:AC34" si="5">IF($L4="Software","","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="AB4" s="21" t="str">
@@ -1770,7 +1775,7 @@
       </c>
       <c r="AD4" s="11"/>
       <c r="AE4" s="21" t="str">
-        <f t="shared" ref="AE3:AK34" si="6">IF($L4="Software","","N/A")</f>
+        <f t="shared" ref="AE4:AK34" si="6">IF($L4="Software","","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="AF4" s="21" t="str">
@@ -17608,7 +17613,7 @@
       <c r="CF98" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Vj5VQf7xGYlyA+0dSq3obptAHLhAi420FQrAn6J6niq7jayN95nf0X1ZSsNJPtEEUQgqhkkRe3Rcz9Ep+AUpng==" saltValue="8JSsT+OV2EXKweOhjYDPdA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3GBw7tA6KTL4QyaRnGFfEeRW6Mt1dZPhWNCISRsZD5hLJZsVPEug+IU+gKZpIc3cV3wDs+MCzfSy1lTwmPAgjw==" saltValue="TKEAzA40/y2uaT4PqGZcDA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="O2:Q1048576 S2:Y1048576">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$L2&lt;&gt;"dataset"</formula>

</xml_diff>